<commit_message>
STACK: Generate Gerbers, format BOM, manage directories
</commit_message>
<xml_diff>
--- a/base/CAM/CSv2.1 CAM Outputs/CAMOutputs/Assembly/cs-main-v2.1_formatted.xlsx
+++ b/base/CAM/CSv2.1 CAM Outputs/CAMOutputs/Assembly/cs-main-v2.1_formatted.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/work-reese/hardware/commonsense/cs-hardware/base/CAM/CSv2.1 CAM Outputs/CAMOutputs/Assembly/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C161CAF-C6DD-0F46-9B7A-BF53006F0002}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7E1CEA5-44F8-DD41-B015-54370C0A92CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9040" yWindow="-28340" windowWidth="51200" windowHeight="28340" xr2:uid="{60C5DCAE-2D49-FC44-9E9E-4B7E9B959C96}"/>
+    <workbookView xWindow="3900" yWindow="2260" windowWidth="28040" windowHeight="17440" xr2:uid="{59362B13-43C8-5C45-B1AE-BE1E85EEB517}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="cs_v2.1" localSheetId="0">Sheet1!$A$1:$Z$42</definedName>
+    <definedName name="cs_v2.1" localSheetId="0">Sheet1!$A$1:$L$42</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +37,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{C29A2DAA-9A06-9D4E-8413-39027D61EEF3}" name="cs_v2.1" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="1" xr16:uid="{8D739017-B83F-094D-9CE1-D9AA9120B1BE}" name="cs_v2.1" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="10000" sourceFile="/Users/work-reese/hardware/commonsense/cs-hardware/base/CAM/CSv2.1 CAM Outputs/CAMOutputs/Assembly/cs_v2.1.csv" tab="0" semicolon="1">
       <textFields count="48">
         <textField/>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="185">
   <si>
     <t>Qty</t>
   </si>
@@ -118,57 +118,15 @@
     <t>MANUFACTURER</t>
   </si>
   <si>
-    <t>MPN</t>
-  </si>
-  <si>
     <t>PART_NO</t>
   </si>
   <si>
-    <t>PART_NUMBER</t>
-  </si>
-  <si>
-    <t>PIN_COUNT</t>
-  </si>
-  <si>
-    <t>POPULARITY</t>
-  </si>
-  <si>
-    <t>PREFIX</t>
-  </si>
-  <si>
-    <t>QUENCH</t>
-  </si>
-  <si>
-    <t>ROHS</t>
-  </si>
-  <si>
-    <t>SERIES</t>
-  </si>
-  <si>
-    <t>SOFTSTART</t>
-  </si>
-  <si>
-    <t>SOURCELIBRARY</t>
-  </si>
-  <si>
     <t>TC</t>
   </si>
   <si>
-    <t>TEMPERATURE_RANGE_HIGH</t>
-  </si>
-  <si>
-    <t>TEMPERATURE_RANGE_LOW</t>
-  </si>
-  <si>
     <t>TOL</t>
   </si>
   <si>
-    <t>TP_SIGNAL_NAME</t>
-  </si>
-  <si>
-    <t>VENDOR</t>
-  </si>
-  <si>
     <t>VOLTAGE</t>
   </si>
   <si>
@@ -259,9 +217,6 @@
     <t>KOA Speer</t>
   </si>
   <si>
-    <t>KDV06DR510ET</t>
-  </si>
-  <si>
     <t>SR732BTTD1R00D</t>
   </si>
   <si>
@@ -511,21 +466,9 @@
     <t>Micro LED</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>598-8710-307F</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>+100¬∞C</t>
-  </si>
-  <si>
-    <t>-40¬∞C</t>
-  </si>
-  <si>
     <t>DMG3415UFY4Q-7F</t>
   </si>
   <si>
@@ -595,12 +538,6 @@
     <t>MIC94164YCS-TR</t>
   </si>
   <si>
-    <t>MIC94164</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
     <t>MAX77827BEWC+T</t>
   </si>
   <si>
@@ -616,12 +553,6 @@
     <t>Maxim</t>
   </si>
   <si>
-    <t>MAX77827BEWC+</t>
-  </si>
-  <si>
-    <t>Maxim Integrated Products</t>
-  </si>
-  <si>
     <t>NCP708MU330TAG</t>
   </si>
   <si>
@@ -652,9 +583,6 @@
     <t>1A Schottky Barrier Rectifier.</t>
   </si>
   <si>
-    <t>Diodes Inc</t>
-  </si>
-  <si>
     <t>SENSOR-SI7006</t>
   </si>
   <si>
@@ -697,7 +625,7 @@
     <t>U3</t>
   </si>
   <si>
-    <t>Dual circuit SPDT Switch IC with very low on-resistance</t>
+    <t>0.3 Ohm Dual SPDT Analog Switch Dual-Channel 2:1 Multiplexer/Demultiplexer</t>
   </si>
   <si>
     <t>Texas Instruments</t>
@@ -715,10 +643,13 @@
     <t>1 Gbit flash storage, programmable through SPI, Dual SPI or Quad SPI, manufactured by Winbond.</t>
   </si>
   <si>
-    <t>Winbond_2020-02-06</t>
-  </si>
-  <si>
-    <t>Winbond</t>
+    <t>W25N01GVZEIG TR</t>
+  </si>
+  <si>
+    <t>Diodes Inc.</t>
+  </si>
+  <si>
+    <t>Yageo</t>
   </si>
 </sst>
 </file>
@@ -776,7 +707,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="cs_v2.1" connectionId="1" xr16:uid="{5B3745B8-CD32-E440-BBEB-916DCAEB3971}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="cs_v2.1" connectionId="1" xr16:uid="{952DDCC7-7C29-6F41-AF87-5609032F89E3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1075,11 +1006,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C63B7E1-B4D3-A24E-A953-15D201D41D44}">
-  <dimension ref="A1:Y42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ED734BE-102B-AE4C-8CEA-26732FD516A5}">
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1090,25 +1021,13 @@
     <col min="5" max="5" width="70" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="80.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="26" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1142,137 +1061,89 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="H2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="E3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="F3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="G3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="H3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="G4" t="s">
-        <v>42</v>
+        <v>28</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
       </c>
       <c r="I4" t="s">
-        <v>43</v>
-      </c>
-      <c r="S4" t="s">
-        <v>44</v>
-      </c>
-      <c r="V4" s="1">
+        <v>30</v>
+      </c>
+      <c r="J4" s="1">
         <v>0.1</v>
       </c>
-      <c r="Y4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="K4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1280,430 +1151,409 @@
         <v>0.24</v>
       </c>
       <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
         <v>46</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
         <v>47</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" t="s">
         <v>48</v>
       </c>
-      <c r="F5" t="s">
+      <c r="I8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K8" t="s">
         <v>49</v>
       </c>
-      <c r="G5" t="s">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
         <v>50</v>
       </c>
-      <c r="H5" t="s">
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" t="s">
         <v>51</v>
       </c>
-      <c r="I5" t="s">
-        <v>51</v>
-      </c>
-      <c r="V5" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" t="s">
         <v>52</v>
       </c>
-      <c r="F6" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H6" t="s">
-        <v>54</v>
-      </c>
-      <c r="I6" t="s">
-        <v>55</v>
-      </c>
-      <c r="V6" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" t="s">
-        <v>50</v>
-      </c>
-      <c r="H7" t="s">
-        <v>60</v>
-      </c>
-      <c r="I7" t="s">
-        <v>60</v>
-      </c>
-      <c r="V7" s="1">
+      <c r="J9" s="1">
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I8" t="s">
-        <v>63</v>
-      </c>
-      <c r="S8" t="s">
-        <v>44</v>
-      </c>
-      <c r="V8" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" t="s">
-        <v>66</v>
-      </c>
-      <c r="F9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G9" t="s">
-        <v>50</v>
-      </c>
-      <c r="H9" t="s">
-        <v>67</v>
-      </c>
-      <c r="I9" t="s">
-        <v>67</v>
-      </c>
-      <c r="V9" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="G10" t="s">
-        <v>42</v>
+        <v>28</v>
+      </c>
+      <c r="H10" t="s">
+        <v>55</v>
       </c>
       <c r="I10" t="s">
-        <v>70</v>
-      </c>
-      <c r="S10" t="s">
-        <v>44</v>
-      </c>
-      <c r="V10" s="1">
+        <v>30</v>
+      </c>
+      <c r="J10" s="1">
         <v>0.1</v>
       </c>
-      <c r="Y10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="K10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="F11" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="G11" t="s">
-        <v>42</v>
+        <v>28</v>
+      </c>
+      <c r="H11" t="s">
+        <v>60</v>
       </c>
       <c r="I11" t="s">
-        <v>75</v>
-      </c>
-      <c r="S11" t="s">
-        <v>76</v>
-      </c>
-      <c r="V11" s="1">
+        <v>61</v>
+      </c>
+      <c r="J11" s="1">
         <v>0.1</v>
       </c>
-      <c r="Y11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="K11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="D12" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="E12" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="F12" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="G12" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" t="s">
+        <v>65</v>
+      </c>
+      <c r="I12" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" t="s">
         <v>42</v>
       </c>
-      <c r="I12" t="s">
-        <v>80</v>
-      </c>
-      <c r="S12" t="s">
-        <v>44</v>
-      </c>
-      <c r="V12" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>81</v>
-      </c>
-      <c r="C13" t="s">
-        <v>57</v>
-      </c>
       <c r="D13" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E13" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="F13" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="G13" t="s">
-        <v>50</v>
-      </c>
-      <c r="I13" t="s">
-        <v>83</v>
-      </c>
-      <c r="V13" s="2">
+        <v>36</v>
+      </c>
+      <c r="H13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J13" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="D14" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E14" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="F14" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="G14" t="s">
-        <v>50</v>
-      </c>
-      <c r="I14" t="s">
-        <v>85</v>
-      </c>
-      <c r="V14" s="1">
+        <v>36</v>
+      </c>
+      <c r="H14" t="s">
+        <v>70</v>
+      </c>
+      <c r="J14" s="1">
         <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="E15" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="F15" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="G15" t="s">
-        <v>42</v>
+        <v>28</v>
+      </c>
+      <c r="H15" t="s">
+        <v>73</v>
       </c>
       <c r="I15" t="s">
-        <v>88</v>
-      </c>
-      <c r="S15" t="s">
-        <v>76</v>
-      </c>
-      <c r="V15" s="1">
+        <v>61</v>
+      </c>
+      <c r="J15" s="1">
         <v>0.1</v>
       </c>
-      <c r="Y15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="K15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="E16" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="F16" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="G16" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="H16" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="I16" t="s">
-        <v>88</v>
-      </c>
-      <c r="S16" t="s">
+        <v>61</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" t="s">
         <v>76</v>
       </c>
-      <c r="V16" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C17" t="s">
-        <v>90</v>
-      </c>
-      <c r="D17" t="s">
-        <v>90</v>
-      </c>
-      <c r="E17" t="s">
-        <v>91</v>
-      </c>
       <c r="F17" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="G17" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="H17" t="s">
-        <v>94</v>
-      </c>
-      <c r="I17" t="s">
-        <v>94</v>
-      </c>
-      <c r="P17" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1711,66 +1561,63 @@
         <v>2.21</v>
       </c>
       <c r="C18" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="E18" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="F18" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="G18" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="H18" t="s">
-        <v>97</v>
-      </c>
-      <c r="I18" t="s">
-        <v>97</v>
-      </c>
-      <c r="V18" s="2">
+        <v>82</v>
+      </c>
+      <c r="J18" s="2">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="E19" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="F19" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="G19" t="s">
-        <v>42</v>
+        <v>28</v>
+      </c>
+      <c r="H19" t="s">
+        <v>85</v>
       </c>
       <c r="I19" t="s">
-        <v>100</v>
-      </c>
-      <c r="S19" t="s">
-        <v>76</v>
-      </c>
-      <c r="V19" s="1">
+        <v>61</v>
+      </c>
+      <c r="J19" s="1">
         <v>0.1</v>
       </c>
-      <c r="Y19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="K19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1778,28 +1625,28 @@
         <v>330</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="D20" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E20" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="F20" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="G20" t="s">
-        <v>50</v>
-      </c>
-      <c r="I20" t="s">
-        <v>102</v>
-      </c>
-      <c r="V20" s="1">
+        <v>36</v>
+      </c>
+      <c r="H20" t="s">
+        <v>87</v>
+      </c>
+      <c r="J20" s="1">
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1807,159 +1654,156 @@
         <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E21" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="F21" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="G21" t="s">
-        <v>50</v>
-      </c>
-      <c r="I21" t="s">
-        <v>104</v>
-      </c>
-      <c r="V21" s="1">
+        <v>36</v>
+      </c>
+      <c r="H21" t="s">
+        <v>89</v>
+      </c>
+      <c r="J21" s="1">
         <v>0.05</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="D22" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E22" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="F22" t="s">
+        <v>35</v>
+      </c>
+      <c r="G22" t="s">
+        <v>36</v>
+      </c>
+      <c r="H22" t="s">
+        <v>92</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" t="s">
+        <v>94</v>
+      </c>
+      <c r="F23" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23" t="s">
+        <v>28</v>
+      </c>
+      <c r="H23" t="s">
+        <v>95</v>
+      </c>
+      <c r="I23" t="s">
+        <v>30</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" t="s">
+        <v>97</v>
+      </c>
+      <c r="F24" t="s">
+        <v>27</v>
+      </c>
+      <c r="G24" t="s">
+        <v>184</v>
+      </c>
+      <c r="H24" t="s">
+        <v>98</v>
+      </c>
+      <c r="I24" t="s">
+        <v>30</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K24" t="s">
         <v>49</v>
       </c>
-      <c r="G22" t="s">
-        <v>50</v>
-      </c>
-      <c r="I22" t="s">
-        <v>107</v>
-      </c>
-      <c r="V22" s="1">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" t="s">
+        <v>100</v>
+      </c>
+      <c r="F25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G25" t="s">
+        <v>36</v>
+      </c>
+      <c r="H25" t="s">
+        <v>101</v>
+      </c>
+      <c r="J25" s="1">
         <v>0.05</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
-        <v>108</v>
-      </c>
-      <c r="C23" t="s">
-        <v>77</v>
-      </c>
-      <c r="D23" t="s">
-        <v>78</v>
-      </c>
-      <c r="E23" t="s">
-        <v>109</v>
-      </c>
-      <c r="F23" t="s">
-        <v>41</v>
-      </c>
-      <c r="G23" t="s">
-        <v>42</v>
-      </c>
-      <c r="I23" t="s">
-        <v>110</v>
-      </c>
-      <c r="S23" t="s">
-        <v>44</v>
-      </c>
-      <c r="V23" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="Y23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>1</v>
-      </c>
-      <c r="B24" t="s">
-        <v>111</v>
-      </c>
-      <c r="C24" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" t="s">
-        <v>39</v>
-      </c>
-      <c r="E24" t="s">
-        <v>112</v>
-      </c>
-      <c r="F24" t="s">
-        <v>41</v>
-      </c>
-      <c r="G24" t="s">
-        <v>42</v>
-      </c>
-      <c r="I24" t="s">
-        <v>113</v>
-      </c>
-      <c r="S24" t="s">
-        <v>44</v>
-      </c>
-      <c r="V24" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>1</v>
-      </c>
-      <c r="B25" t="s">
-        <v>114</v>
-      </c>
-      <c r="C25" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" t="s">
-        <v>58</v>
-      </c>
-      <c r="E25" t="s">
-        <v>115</v>
-      </c>
-      <c r="F25" t="s">
-        <v>49</v>
-      </c>
-      <c r="G25" t="s">
-        <v>50</v>
-      </c>
-      <c r="H25" t="s">
-        <v>116</v>
-      </c>
-      <c r="I25" t="s">
-        <v>116</v>
-      </c>
-      <c r="V25" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2</v>
       </c>
@@ -1967,477 +1811,411 @@
         <v>590</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="D26" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E26" t="s">
+        <v>102</v>
+      </c>
+      <c r="F26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G26" t="s">
+        <v>36</v>
+      </c>
+      <c r="H26" t="s">
+        <v>103</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27" t="s">
+        <v>104</v>
+      </c>
+      <c r="D27" t="s">
+        <v>105</v>
+      </c>
+      <c r="E27" t="s">
+        <v>106</v>
+      </c>
+      <c r="F27" t="s">
+        <v>107</v>
+      </c>
+      <c r="H27" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" t="s">
+        <v>108</v>
+      </c>
+      <c r="D28" t="s">
+        <v>109</v>
+      </c>
+      <c r="E28" t="s">
+        <v>110</v>
+      </c>
+      <c r="F28" t="s">
+        <v>111</v>
+      </c>
+      <c r="H28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>113</v>
+      </c>
+      <c r="C29" t="s">
+        <v>113</v>
+      </c>
+      <c r="D29" t="s">
+        <v>114</v>
+      </c>
+      <c r="E29" t="s">
+        <v>115</v>
+      </c>
+      <c r="F29" t="s">
+        <v>116</v>
+      </c>
+      <c r="G29" t="s">
         <v>117</v>
       </c>
-      <c r="F26" t="s">
-        <v>49</v>
-      </c>
-      <c r="G26" t="s">
-        <v>50</v>
-      </c>
-      <c r="I26" t="s">
+      <c r="H29" t="s">
         <v>118</v>
       </c>
-      <c r="V26" s="1">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s">
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
         <v>119</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C30" t="s">
         <v>119</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D30" t="s">
         <v>120</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E30" t="s">
         <v>121</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F30" t="s">
         <v>122</v>
       </c>
-      <c r="I27" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="H30" t="s">
         <v>123</v>
       </c>
-      <c r="C28" t="s">
-        <v>123</v>
-      </c>
-      <c r="D28" t="s">
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
         <v>124</v>
       </c>
-      <c r="E28" t="s">
+      <c r="C31" t="s">
+        <v>124</v>
+      </c>
+      <c r="D31" t="s">
         <v>125</v>
       </c>
-      <c r="F28" t="s">
+      <c r="E31" t="s">
         <v>126</v>
       </c>
-      <c r="I28" t="s">
+      <c r="F31" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>1</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="G31" t="s">
+        <v>183</v>
+      </c>
+      <c r="H31" t="s">
         <v>128</v>
       </c>
-      <c r="C29" t="s">
-        <v>128</v>
-      </c>
-      <c r="D29" t="s">
-        <v>129</v>
-      </c>
-      <c r="E29" t="s">
-        <v>130</v>
-      </c>
-      <c r="F29" t="s">
-        <v>131</v>
-      </c>
-      <c r="G29" t="s">
-        <v>132</v>
-      </c>
-      <c r="H29" t="s">
-        <v>133</v>
-      </c>
-      <c r="I29" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>1</v>
-      </c>
-      <c r="B30" t="s">
-        <v>134</v>
-      </c>
-      <c r="C30" t="s">
-        <v>134</v>
-      </c>
-      <c r="D30" t="s">
-        <v>135</v>
-      </c>
-      <c r="E30" t="s">
-        <v>136</v>
-      </c>
-      <c r="F30" t="s">
-        <v>137</v>
-      </c>
-      <c r="H30" t="s">
-        <v>139</v>
-      </c>
-      <c r="I30" t="s">
-        <v>139</v>
-      </c>
-      <c r="M30" t="s">
-        <v>140</v>
-      </c>
-      <c r="O30" t="s">
-        <v>138</v>
-      </c>
-      <c r="T30" t="s">
-        <v>141</v>
-      </c>
-      <c r="U30" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>1</v>
-      </c>
-      <c r="B31" t="s">
-        <v>143</v>
-      </c>
-      <c r="C31" t="s">
-        <v>143</v>
-      </c>
-      <c r="D31" t="s">
-        <v>144</v>
-      </c>
-      <c r="E31" t="s">
-        <v>145</v>
-      </c>
-      <c r="F31" t="s">
-        <v>146</v>
-      </c>
-      <c r="H31" t="s">
-        <v>147</v>
-      </c>
-      <c r="I31" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="C32" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="D32" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="E32" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="F32" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="H32" t="s">
-        <v>152</v>
-      </c>
-      <c r="I32" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="C33" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="D33" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="E33" t="s">
-        <v>154</v>
-      </c>
-      <c r="I33" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+      <c r="H33" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="C34" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="D34" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="E34" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="F34" t="s">
-        <v>158</v>
-      </c>
-      <c r="I34" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+      <c r="H34" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>3</v>
       </c>
       <c r="B35" t="s">
+        <v>141</v>
+      </c>
+      <c r="C35" t="s">
+        <v>141</v>
+      </c>
+      <c r="D35" t="s">
+        <v>142</v>
+      </c>
+      <c r="E35" t="s">
+        <v>143</v>
+      </c>
+      <c r="F35" t="s">
+        <v>144</v>
+      </c>
+      <c r="G35" t="s">
+        <v>145</v>
+      </c>
+      <c r="H35" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>147</v>
+      </c>
+      <c r="C36" t="s">
+        <v>147</v>
+      </c>
+      <c r="D36" t="s">
+        <v>148</v>
+      </c>
+      <c r="E36" t="s">
+        <v>149</v>
+      </c>
+      <c r="F36" t="s">
+        <v>150</v>
+      </c>
+      <c r="G36" t="s">
+        <v>151</v>
+      </c>
+      <c r="H36" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>152</v>
+      </c>
+      <c r="C37" t="s">
+        <v>153</v>
+      </c>
+      <c r="D37" t="s">
+        <v>154</v>
+      </c>
+      <c r="E37" t="s">
+        <v>155</v>
+      </c>
+      <c r="F37" t="s">
+        <v>156</v>
+      </c>
+      <c r="G37" t="s">
+        <v>157</v>
+      </c>
+      <c r="H37" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>158</v>
+      </c>
+      <c r="C38" t="s">
+        <v>158</v>
+      </c>
+      <c r="D38" t="s">
+        <v>159</v>
+      </c>
+      <c r="E38" t="s">
         <v>160</v>
       </c>
-      <c r="C35" t="s">
-        <v>160</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="F38" t="s">
         <v>161</v>
       </c>
-      <c r="E35" t="s">
+      <c r="H38" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39" t="s">
         <v>162</v>
       </c>
-      <c r="F35" t="s">
+      <c r="C39" t="s">
+        <v>162</v>
+      </c>
+      <c r="D39" t="s">
         <v>163</v>
       </c>
-      <c r="G35" t="s">
+      <c r="E39" t="s">
         <v>164</v>
       </c>
-      <c r="H35" t="s">
+      <c r="F39" t="s">
         <v>165</v>
       </c>
-      <c r="I35" t="s">
-        <v>165</v>
-      </c>
-      <c r="J35" t="s">
+      <c r="G39" t="s">
         <v>166</v>
       </c>
-      <c r="N35" t="s">
+      <c r="H39" t="s">
         <v>167</v>
       </c>
-      <c r="Q35" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>1</v>
-      </c>
-      <c r="B36" t="s">
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40" t="s">
         <v>168</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C40" t="s">
         <v>168</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D40" t="s">
         <v>169</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E40" t="s">
         <v>170</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F40" t="s">
         <v>171</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H40" t="s">
         <v>172</v>
       </c>
-      <c r="H36" t="s">
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41" t="s">
         <v>173</v>
       </c>
-      <c r="I36" t="s">
-        <v>168</v>
-      </c>
-      <c r="X36" t="s">
+      <c r="C41" t="s">
+        <v>173</v>
+      </c>
+      <c r="D41" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>1</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="E41" t="s">
         <v>175</v>
       </c>
-      <c r="C37" t="s">
+      <c r="F41" t="s">
         <v>176</v>
       </c>
-      <c r="D37" t="s">
+      <c r="G41" t="s">
         <v>177</v>
       </c>
-      <c r="E37" t="s">
+      <c r="H41" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
         <v>178</v>
       </c>
-      <c r="F37" t="s">
+      <c r="C42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D42" t="s">
         <v>179</v>
       </c>
-      <c r="G37" t="s">
+      <c r="E42" t="s">
         <v>180</v>
       </c>
-      <c r="H37" t="s">
-        <v>175</v>
-      </c>
-      <c r="I37" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="38" spans="1:24" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>1</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="F42" t="s">
         <v>181</v>
       </c>
-      <c r="C38" t="s">
-        <v>181</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="H42" t="s">
         <v>182</v>
-      </c>
-      <c r="E38" t="s">
-        <v>183</v>
-      </c>
-      <c r="F38" t="s">
-        <v>184</v>
-      </c>
-      <c r="I38" t="s">
-        <v>181</v>
-      </c>
-      <c r="X38" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>1</v>
-      </c>
-      <c r="B39" t="s">
-        <v>186</v>
-      </c>
-      <c r="C39" t="s">
-        <v>186</v>
-      </c>
-      <c r="D39" t="s">
-        <v>187</v>
-      </c>
-      <c r="E39" t="s">
-        <v>188</v>
-      </c>
-      <c r="F39" t="s">
-        <v>189</v>
-      </c>
-      <c r="G39" t="s">
-        <v>190</v>
-      </c>
-      <c r="H39" t="s">
-        <v>191</v>
-      </c>
-      <c r="I39" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>1</v>
-      </c>
-      <c r="B40" t="s">
-        <v>192</v>
-      </c>
-      <c r="C40" t="s">
-        <v>192</v>
-      </c>
-      <c r="D40" t="s">
-        <v>193</v>
-      </c>
-      <c r="E40" t="s">
-        <v>194</v>
-      </c>
-      <c r="F40" t="s">
-        <v>195</v>
-      </c>
-      <c r="I40" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>1</v>
-      </c>
-      <c r="B41" t="s">
-        <v>197</v>
-      </c>
-      <c r="C41" t="s">
-        <v>197</v>
-      </c>
-      <c r="D41" t="s">
-        <v>198</v>
-      </c>
-      <c r="E41" t="s">
-        <v>199</v>
-      </c>
-      <c r="F41" t="s">
-        <v>200</v>
-      </c>
-      <c r="G41" t="s">
-        <v>201</v>
-      </c>
-      <c r="H41" t="s">
-        <v>197</v>
-      </c>
-      <c r="I41" t="s">
-        <v>197</v>
-      </c>
-      <c r="K41">
-        <v>10</v>
-      </c>
-      <c r="X41" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>1</v>
-      </c>
-      <c r="B42" t="s">
-        <v>202</v>
-      </c>
-      <c r="C42" t="s">
-        <v>202</v>
-      </c>
-      <c r="D42" t="s">
-        <v>203</v>
-      </c>
-      <c r="E42" t="s">
-        <v>204</v>
-      </c>
-      <c r="F42" t="s">
-        <v>205</v>
-      </c>
-      <c r="H42" t="s">
-        <v>202</v>
-      </c>
-      <c r="I42" t="s">
-        <v>202</v>
-      </c>
-      <c r="R42" t="s">
-        <v>206</v>
-      </c>
-      <c r="X42" t="s">
-        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>